<commit_message>
Goodluck to you git add .!
</commit_message>
<xml_diff>
--- a/Note.xlsx
+++ b/Note.xlsx
@@ -1,21 +1,95 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Difficulity</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Problem components</t>
+  </si>
+  <si>
+    <t>Solution ideas</t>
+  </si>
+  <si>
+    <t>Solution component</t>
+  </si>
+  <si>
+    <t>739. Daily Temperatures</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>Array, Stack</t>
+  </si>
+  <si>
+    <t>- Give an integer array of temperatures
+- Return an array which array[i] is number of day need to wait for warmer temperature</t>
+  </si>
+  <si>
+    <t>- Two</t>
+  </si>
+  <si>
+    <t>496. Next Greater Element I</t>
+  </si>
+  <si>
+    <t>Easy</t>
+  </si>
+  <si>
+    <t>- Give two integer arrays arr1 and arr2
+- arr1 is a sub array of arr2
+- Return an array which arr[i] is a next greater of arr1[i] in arr2
+- If have no greater value, fill -1</t>
+  </si>
+  <si>
+    <t>- Two loops, one for choose element in arr1, one to check in arr2
+- Use a flag to check if arr1 element is found and start to check greater
+--&gt; Time: O(n^2)
+- Use a hash map to store arr2 value and index to get faster
+--&gt; Time: O(n^2) (97% beats)</t>
+  </si>
+  <si>
+    <t>- Iterate over arr2, store all value which small than previous value to a stack
+- If encounter a value bigger than top value of stack, pop it and put to a hash map to store its greater value
+- Finally, we will iterate over arr1 and get value from hashmap for output
+--&gt; Time: O(arr1.length + arr2.length + arr2.length) -&gt; O(n)
+- Why don't we use array ans directly instead of use a map? --&gt; Because we don't know index of current element.
+- When we encounter a value which bigger than top stack value, we will pop all stack? No, we will pop if that value bigger than current top stack.</t>
+  </si>
+  <si>
+    <t>- Two loops, one for day, one for check temperature
+--&gt; (TLE)
+- F2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -23,16 +97,45 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <scheme val="major"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,18 +143,424 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="49">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor auto="1"/>
+          <bgColor rgb="FFFDF6B3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9966"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFFCC"/>
+      <color rgb="FFFF9966"/>
+      <color rgb="FFFF8181"/>
+      <color rgb="FFFFFF99"/>
+      <color rgb="FFFDF6B3"/>
+      <color rgb="FFEFEEC1"/>
+    </mruColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +607,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +642,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +850,507 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="29.7265625" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="26.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.6328125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="68.26953125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="71.81640625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="41" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="29.7265625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="20" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="240.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" ht="74" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="1"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="1"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="1"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="1"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="1"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="1"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="1"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="1"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="1"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A46" s="1"/>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A47" s="1"/>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A48" s="1"/>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A1:G1048576">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>$B1="Hard"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$B1="Medium"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="3">
+      <formula>$B1="Easy"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Good luck git add .!
</commit_message>
<xml_diff>
--- a/Note.xlsx
+++ b/Note.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EADFA1-4E1D-4A13-847C-B4009E2B9773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-144" yWindow="12852" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -80,15 +81,19 @@
 - When we encounter a value which bigger than top stack value, we will pop all stack? No, we will pop if that value bigger than current top stack.</t>
   </si>
   <si>
-    <t>- Two loops, one for day, one for check temperature
+    <t xml:space="preserve">- Brute force
+- Two loops, one for day, one for check temperature
 --&gt; (TLE)
-- F2</t>
+- Iterate over the input array
+- keep the index and value of value which small than its previous value
+- while the value bigger than stack.peek(), pop the stack and assign index to answer array.
+--&gt; O(2*N) An easier way to think about this is that in the worst case, every element will be pushed and popped once. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -186,7 +191,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="49">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -198,339 +203,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9966"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor auto="1"/>
-          <bgColor rgb="FFFDF6B3"/>
         </patternFill>
       </fill>
     </dxf>
@@ -565,9 +237,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -605,9 +277,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -642,7 +314,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -677,7 +349,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -850,27 +522,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="29.7265625" defaultRowHeight="18.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="29.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.54296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.36328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="57.6328125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="68.26953125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="71.81640625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="57.5703125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="68.28515625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="71.85546875" style="6" customWidth="1"/>
     <col min="7" max="7" width="41" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="29.7265625" style="2"/>
+    <col min="8" max="16384" width="29.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" ht="20" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="4" customFormat="1" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -893,7 +565,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="240.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="243.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -912,7 +584,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="74" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="225" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -933,7 +605,7 @@
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -942,7 +614,7 @@
       <c r="F4" s="5"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -951,7 +623,7 @@
       <c r="F5" s="5"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -960,7 +632,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -969,7 +641,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -978,7 +650,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -987,7 +659,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -996,7 +668,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1005,7 +677,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1014,7 +686,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1023,7 +695,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1032,7 +704,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1041,7 +713,7 @@
       <c r="F15" s="5"/>
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1050,7 +722,7 @@
       <c r="F16" s="5"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1059,7 +731,7 @@
       <c r="F17" s="5"/>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1068,7 +740,7 @@
       <c r="F18" s="5"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1077,7 +749,7 @@
       <c r="F19" s="5"/>
       <c r="G19" s="1"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1086,7 +758,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1095,7 +767,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="1"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1104,7 +776,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="1"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1113,7 +785,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="1"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -1122,7 +794,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1131,7 +803,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1140,7 +812,7 @@
       <c r="F26" s="5"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1149,7 +821,7 @@
       <c r="F27" s="5"/>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1158,7 +830,7 @@
       <c r="F28" s="5"/>
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1167,7 +839,7 @@
       <c r="F29" s="5"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1176,7 +848,7 @@
       <c r="F30" s="5"/>
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1185,7 +857,7 @@
       <c r="F31" s="5"/>
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1194,7 +866,7 @@
       <c r="F32" s="5"/>
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1203,7 +875,7 @@
       <c r="F33" s="5"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1212,7 +884,7 @@
       <c r="F34" s="5"/>
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1221,7 +893,7 @@
       <c r="F35" s="5"/>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1230,7 +902,7 @@
       <c r="F36" s="5"/>
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1239,7 +911,7 @@
       <c r="F37" s="5"/>
       <c r="G37" s="1"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1248,7 +920,7 @@
       <c r="F38" s="5"/>
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1257,7 +929,7 @@
       <c r="F39" s="5"/>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1266,7 +938,7 @@
       <c r="F40" s="5"/>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1275,7 +947,7 @@
       <c r="F41" s="5"/>
       <c r="G41" s="1"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1284,7 +956,7 @@
       <c r="F42" s="5"/>
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1293,7 +965,7 @@
       <c r="F43" s="5"/>
       <c r="G43" s="1"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1302,7 +974,7 @@
       <c r="F44" s="5"/>
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1311,7 +983,7 @@
       <c r="F45" s="5"/>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1320,7 +992,7 @@
       <c r="F46" s="5"/>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1329,7 +1001,7 @@
       <c r="F47" s="5"/>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>

</xml_diff>